<commit_message>
test edits to source data
</commit_message>
<xml_diff>
--- a/data-files/assessments.xlsx
+++ b/data-files/assessments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcarlson\Desktop\Repos\ilgisa-2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcarlson\Desktop\Repos\ilgisa-2022\data-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
   <si>
     <t>01-06-100-001</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>LR003</t>
+  </si>
+  <si>
+    <t>LR022</t>
   </si>
 </sst>
 </file>
@@ -298,14 +301,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E30" totalsRowShown="0">
-  <autoFilter ref="A1:E30">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="0011"/>
-        <filter val="0040"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E30"/>
   <tableColumns count="5">
     <tableColumn id="1" name="parcel_number"/>
     <tableColumn id="2" name="property_class" dataDxfId="1"/>
@@ -583,7 +579,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -645,7 +641,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -658,8 +654,11 @@
       <c r="D4" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -671,6 +670,9 @@
       </c>
       <c r="D5" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -690,7 +692,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -703,8 +705,11 @@
       <c r="D7" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -717,8 +722,11 @@
       <c r="D8" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -730,6 +738,9 @@
       </c>
       <c r="D9" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -800,7 +811,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -812,6 +823,9 @@
       </c>
       <c r="D14" s="2" t="s">
         <v>49</v>
+      </c>
+      <c r="E14" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -848,7 +862,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -861,8 +875,11 @@
       <c r="D17" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="E17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -874,6 +891,9 @@
       </c>
       <c r="D18" s="2" t="s">
         <v>53</v>
+      </c>
+      <c r="E18" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -890,10 +910,10 @@
         <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -906,8 +926,11 @@
       <c r="D20" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="E20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -920,8 +943,11 @@
       <c r="D21" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="E21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -933,6 +959,9 @@
       </c>
       <c r="D22" s="2" t="s">
         <v>57</v>
+      </c>
+      <c r="E22" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -949,7 +978,7 @@
         <v>58</v>
       </c>
       <c r="E23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1003,7 +1032,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1015,6 +1044,9 @@
       </c>
       <c r="D27" s="2" t="s">
         <v>62</v>
+      </c>
+      <c r="E27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1051,7 +1083,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1063,6 +1095,9 @@
       </c>
       <c r="D30" s="2" t="s">
         <v>65</v>
+      </c>
+      <c r="E30" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>